<commit_message>
added local and remote driver factory. Added suirefire plugin
</commit_message>
<xml_diff>
--- a/Demo.xlsx
+++ b/Demo.xlsx
@@ -362,7 +362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>